<commit_message>
update data depot with new download files and pre 2000 data
</commit_message>
<xml_diff>
--- a/data/download/Demographic Snapshot - Longest Prison Terms.xlsx
+++ b/data/download/Demographic Snapshot - Longest Prison Terms.xlsx
@@ -1,25 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\EPelletier\Desktop\Plane Work\DOWNLOADABLE DATA FILES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bchartof/Projects/long-sentences/data/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108"/>
+    <workbookView xWindow="4180" yWindow="7360" windowWidth="23040" windowHeight="9100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>AK</t>
   </si>
@@ -153,58 +161,67 @@
     <t>WY</t>
   </si>
   <si>
-    <t>Of state prison population: Percent black</t>
-  </si>
-  <si>
-    <t>Of those serving longest 10% of prison terms: Percent black</t>
-  </si>
-  <si>
-    <t>Number of people incarcerated for half or more of their life</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Of those serving longest 10% of prison terms: </t>
-  </si>
-  <si>
-    <t>Percent incarcerated before age 25</t>
-  </si>
-  <si>
-    <t>Percent currently 55 or older</t>
-  </si>
-  <si>
-    <t>Number of people</t>
-  </si>
-  <si>
     <t>Percent black</t>
   </si>
   <si>
     <t>Percent male</t>
   </si>
   <si>
-    <t>Percent convicted of violent offenses</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Of those serving 10 or more years: Percent who are black men incarcerated before age 25</t>
-  </si>
-  <si>
-    <t>Of those serving longest 10% of prison terms who were incarcerated before age 25:</t>
-  </si>
-  <si>
-    <t>All Available States</t>
-  </si>
-  <si>
-    <t>Most recent available</t>
+    <t>All states analyzed</t>
+  </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>National Corrections Reporting Program</t>
+  </si>
+  <si>
+    <t>https://www.bjs.gov/index.cfm?ty=dcdetail&amp;iid=268</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>OF STATE PRISON POPULATION, PERCENT BLACK</t>
+  </si>
+  <si>
+    <t>OF THOSE SERVING LONGEST 10% OF PRISON TERMS, PERCENT BLACK</t>
+  </si>
+  <si>
+    <t>PEOPLE INCARCERATED FOR HALF OF THEIR LIFE OR MORE</t>
+  </si>
+  <si>
+    <t>OF THOSE SERVING LONGEST 10% OF PRISON TERMS</t>
+  </si>
+  <si>
+    <t>Share incarcerated before age 25</t>
+  </si>
+  <si>
+    <t>Share currently 55 or older</t>
+  </si>
+  <si>
+    <t>People</t>
+  </si>
+  <si>
+    <t>Share convicted of violent offenses</t>
+  </si>
+  <si>
+    <t>OF THOSE SERVING 10 OR MORE YEARS:</t>
+  </si>
+  <si>
+    <t>Share who are black men incarcerated before age 25</t>
+  </si>
+  <si>
+    <t>OF THOSE SERVING LONGEST 10% OF PRISON TERMS WHO WERE INCARCERATED BEFORE AGE 25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -704,7 +721,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -714,8 +731,12 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1073,79 +1094,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="7" width="20" customWidth="1"/>
-    <col min="8" max="11" width="18.88671875" customWidth="1"/>
+    <col min="8" max="11" width="18.83203125" customWidth="1"/>
     <col min="12" max="12" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="40.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1167,23 +1190,23 @@
       <c r="G3" s="3">
         <v>0.34979423999999998</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
+        <v>44</v>
+      </c>
+      <c r="I3" s="3">
         <v>4.5454546999999998E-2</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <v>1</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="3">
         <v>0.93181818999999999</v>
-      </c>
-      <c r="K3" s="2">
-        <v>44</v>
       </c>
       <c r="L3" s="3">
         <v>2.0648967000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1205,23 +1228,23 @@
       <c r="G4" s="3">
         <v>0.30502793</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
+        <v>1101</v>
+      </c>
+      <c r="I4" s="3">
         <v>0.77384198000000004</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>0.99545866000000005</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>0.93642144999999999</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1101</v>
       </c>
       <c r="L4" s="3">
         <v>0.28429925</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1243,23 +1266,23 @@
       <c r="G5" s="3">
         <v>0.26388889999999998</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
+        <v>1238</v>
+      </c>
+      <c r="I5" s="3">
         <v>0.21567043999999999</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>0.97011309999999995</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>0.85218095999999999</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1238</v>
       </c>
       <c r="L5" s="3">
         <v>6.6822976000000006E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1281,23 +1304,23 @@
       <c r="G6" s="3">
         <v>0.37783280000000002</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
+        <v>5924</v>
+      </c>
+      <c r="I6" s="3">
         <v>0.41255909000000002</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <v>0.97974342000000003</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <v>0.97974002000000004</v>
-      </c>
-      <c r="K6" s="2">
-        <v>5924</v>
       </c>
       <c r="L6" s="3">
         <v>0.12998433000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1319,23 +1342,23 @@
       <c r="G7" s="3">
         <v>0.35584417000000002</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
+        <v>598</v>
+      </c>
+      <c r="I7" s="3">
         <v>0.29431437999999999</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <v>0.97491640000000002</v>
       </c>
-      <c r="J7" s="3">
+      <c r="K7" s="3">
         <v>0.94983280000000003</v>
-      </c>
-      <c r="K7" s="2">
-        <v>598</v>
       </c>
       <c r="L7" s="3">
         <v>8.2180955E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1357,23 +1380,23 @@
       <c r="G8" s="3">
         <v>0.2254902</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
+        <v>133</v>
+      </c>
+      <c r="I8" s="3">
         <v>0.97744363999999995</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <v>0.94736843999999998</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <v>0.92481201999999996</v>
-      </c>
-      <c r="K8" s="2">
-        <v>133</v>
       </c>
       <c r="L8" s="3">
         <v>0.23863635999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1395,23 +1418,23 @@
       <c r="G9" s="3">
         <v>0.44230767999999998</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
+        <v>69</v>
+      </c>
+      <c r="I9" s="3">
         <v>0.68115943999999995</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <v>0.98550724999999995</v>
       </c>
-      <c r="J9" s="3">
+      <c r="K9" s="3">
         <v>0.89552242000000004</v>
-      </c>
-      <c r="K9" s="2">
-        <v>69</v>
       </c>
       <c r="L9" s="3">
         <v>0.13305897999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1433,23 +1456,23 @@
       <c r="G10" s="3">
         <v>0.37387025000000002</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
+        <v>3855</v>
+      </c>
+      <c r="I10" s="3">
         <v>0.64046692999999999</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <v>0.98287939999999996</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
         <v>0.90609598000000002</v>
-      </c>
-      <c r="K10" s="2">
-        <v>3855</v>
       </c>
       <c r="L10" s="3">
         <v>0.21729279000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1471,23 +1494,23 @@
       <c r="G11" s="3">
         <v>0.33581948</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
+        <v>2130</v>
+      </c>
+      <c r="I11" s="3">
         <v>0.76760565999999997</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <v>0.97042251000000002</v>
       </c>
-      <c r="J11" s="3">
+      <c r="K11" s="3">
         <v>0.95399064</v>
-      </c>
-      <c r="K11" s="2">
-        <v>2130</v>
       </c>
       <c r="L11" s="3">
         <v>0.29139464999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1509,23 +1532,23 @@
       <c r="G12" s="3">
         <v>0.34490481000000001</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
+        <v>326</v>
+      </c>
+      <c r="I12" s="3">
         <v>0.31595093000000002</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <v>0.95398771999999998</v>
       </c>
-      <c r="J12" s="3">
+      <c r="K12" s="3">
         <v>0.91104293000000003</v>
-      </c>
-      <c r="K12" s="2">
-        <v>326</v>
       </c>
       <c r="L12" s="3">
         <v>9.9038458999999995E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1547,23 +1570,23 @@
       <c r="G13" s="3">
         <v>0.24280350000000001</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
+        <v>2181</v>
+      </c>
+      <c r="I13" s="3">
         <v>0.67629528000000005</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <v>0.97524071000000001</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K13" s="3">
         <v>0.93351673999999996</v>
-      </c>
-      <c r="K13" s="2">
-        <v>2181</v>
       </c>
       <c r="L13" s="3">
         <v>0.28396437000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1585,23 +1608,23 @@
       <c r="G14" s="3">
         <v>0.24981871</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
+        <v>755</v>
+      </c>
+      <c r="I14" s="3">
         <v>0.61986755999999998</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <v>0.97615892000000004</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K14" s="3">
         <v>0.82251655999999995</v>
-      </c>
-      <c r="K14" s="2">
-        <v>755</v>
       </c>
       <c r="L14" s="3">
         <v>0.16378466999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1623,23 +1646,23 @@
       <c r="G15" s="3">
         <v>0.33978494999999997</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
+        <v>359</v>
+      </c>
+      <c r="I15" s="3">
         <v>0.52924793999999997</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <v>0.97214484000000001</v>
       </c>
-      <c r="J15" s="3">
+      <c r="K15" s="3">
         <v>0.99164342999999999</v>
-      </c>
-      <c r="K15" s="2">
-        <v>359</v>
       </c>
       <c r="L15" s="3">
         <v>0.19575115000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1661,23 +1684,23 @@
       <c r="G16" s="3">
         <v>0.25977119999999998</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="2">
+        <v>574</v>
+      </c>
+      <c r="I16" s="3">
         <v>0.38850172999999999</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <v>0.97386760000000006</v>
       </c>
-      <c r="J16" s="3">
+      <c r="K16" s="3">
         <v>0.90766548999999996</v>
-      </c>
-      <c r="K16" s="2">
-        <v>574</v>
       </c>
       <c r="L16" s="3">
         <v>9.9386505999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1699,23 +1722,23 @@
       <c r="G17" s="3">
         <v>0.51948053000000005</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="2">
+        <v>335</v>
+      </c>
+      <c r="I17" s="3">
         <v>0.41791045999999998</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <v>0.99402988000000003</v>
       </c>
-      <c r="J17" s="3">
+      <c r="K17" s="3">
         <v>0.97910445999999995</v>
-      </c>
-      <c r="K17" s="2">
-        <v>335</v>
       </c>
       <c r="L17" s="3">
         <v>0.13220733000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1737,23 +1760,23 @@
       <c r="G18" s="3">
         <v>0.33810624</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
+        <v>1142</v>
+      </c>
+      <c r="I18" s="3">
         <v>0.82311732000000004</v>
       </c>
-      <c r="I18" s="3">
+      <c r="J18" s="3">
         <v>0.98949211999999998</v>
       </c>
-      <c r="J18" s="3">
+      <c r="K18" s="3">
         <v>0.99036776999999998</v>
-      </c>
-      <c r="K18" s="2">
-        <v>1142</v>
       </c>
       <c r="L18" s="3">
         <v>0.40549650999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1775,23 +1798,23 @@
       <c r="G19" s="3">
         <v>0.32642486999999998</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
+        <v>47</v>
+      </c>
+      <c r="I19" s="3">
         <v>6.3829786999999999E-2</v>
       </c>
-      <c r="I19" s="3">
+      <c r="J19" s="3">
         <v>0.97872340999999996</v>
       </c>
-      <c r="J19" s="3">
+      <c r="K19" s="3">
         <v>0.89361703000000003</v>
-      </c>
-      <c r="K19" s="2">
-        <v>47</v>
       </c>
       <c r="L19" s="3">
         <v>1.8633541E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1813,23 +1836,23 @@
       <c r="G20" s="3">
         <v>0.42324612</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
+        <v>2051</v>
+      </c>
+      <c r="I20" s="3">
         <v>0.70502191999999997</v>
       </c>
-      <c r="I20" s="3">
+      <c r="J20" s="3">
         <v>0.98391026000000004</v>
       </c>
-      <c r="J20" s="3">
+      <c r="K20" s="3">
         <v>0.94780487000000002</v>
-      </c>
-      <c r="K20" s="2">
-        <v>2051</v>
       </c>
       <c r="L20" s="3">
         <v>0.29252124000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1851,23 +1874,23 @@
       <c r="G21" s="3">
         <v>0.22245762999999999</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="2">
+        <v>360</v>
+      </c>
+      <c r="I21" s="3">
         <v>0.43055555000000001</v>
       </c>
-      <c r="I21" s="3">
+      <c r="J21" s="3">
         <v>0.97222220999999998</v>
       </c>
-      <c r="J21" s="3">
+      <c r="K21" s="3">
         <v>0.91944444000000003</v>
-      </c>
-      <c r="K21" s="2">
-        <v>360</v>
       </c>
       <c r="L21" s="3">
         <v>0.15900132</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1889,23 +1912,23 @@
       <c r="G22" s="3">
         <v>0.31575602000000003</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2">
+        <v>1123</v>
+      </c>
+      <c r="I22" s="3">
         <v>0.62778270000000003</v>
       </c>
-      <c r="I22" s="3">
+      <c r="J22" s="3">
         <v>0.97328585000000001</v>
       </c>
-      <c r="J22" s="3">
+      <c r="K22" s="3">
         <v>0.86553871999999998</v>
-      </c>
-      <c r="K22" s="2">
-        <v>1123</v>
       </c>
       <c r="L22" s="3">
         <v>0.21269411999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1927,23 +1950,23 @@
       <c r="G23" s="3">
         <v>0.29889503000000001</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
+        <v>708</v>
+      </c>
+      <c r="I23" s="3">
         <v>0.83757060999999999</v>
       </c>
-      <c r="I23" s="3">
+      <c r="J23" s="3">
         <v>0.98022598000000005</v>
       </c>
-      <c r="J23" s="3">
+      <c r="K23" s="3">
         <v>0.97033899999999995</v>
-      </c>
-      <c r="K23" s="2">
-        <v>708</v>
       </c>
       <c r="L23" s="3">
         <v>0.30550622999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -1965,23 +1988,23 @@
       <c r="G24" s="3">
         <v>0.43083002999999997</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="2">
+        <v>37</v>
+      </c>
+      <c r="I24" s="3">
         <v>2.7027028000000002E-2</v>
       </c>
-      <c r="I24" s="3">
+      <c r="J24" s="3">
         <v>1</v>
       </c>
-      <c r="J24" s="3">
+      <c r="K24" s="3">
         <v>0.94594592</v>
-      </c>
-      <c r="K24" s="2">
-        <v>37</v>
       </c>
       <c r="L24" s="3">
         <v>3.7037035999999998E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -2003,23 +2026,23 @@
       <c r="G25" s="3">
         <v>0.31601362999999999</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="2">
+        <v>1337</v>
+      </c>
+      <c r="I25" s="3">
         <v>0.72625278999999998</v>
       </c>
-      <c r="I25" s="3">
+      <c r="J25" s="3">
         <v>0.98578905999999999</v>
       </c>
-      <c r="J25" s="3">
+      <c r="K25" s="3">
         <v>0.89154822</v>
-      </c>
-      <c r="K25" s="2">
-        <v>1337</v>
       </c>
       <c r="L25" s="3">
         <v>0.24188034</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
@@ -2041,23 +2064,23 @@
       <c r="G26" s="3">
         <v>0.24260356</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="2">
+        <v>45</v>
+      </c>
+      <c r="I26" s="3">
         <v>4.4444445999999999E-2</v>
       </c>
-      <c r="I26" s="3">
+      <c r="J26" s="3">
         <v>0.95555555999999997</v>
       </c>
-      <c r="J26" s="3">
+      <c r="K26" s="3">
         <v>0.80000000999999998</v>
-      </c>
-      <c r="K26" s="2">
-        <v>45</v>
       </c>
       <c r="L26" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -2079,23 +2102,23 @@
       <c r="G27" s="3">
         <v>0.33955225</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="2">
+        <v>201</v>
+      </c>
+      <c r="I27" s="3">
         <v>0.39800996</v>
       </c>
-      <c r="I27" s="3">
+      <c r="J27" s="3">
         <v>0.97512436000000002</v>
       </c>
-      <c r="J27" s="3">
+      <c r="K27" s="3">
         <v>0.91044778000000004</v>
-      </c>
-      <c r="K27" s="2">
-        <v>201</v>
       </c>
       <c r="L27" s="3">
         <v>0.14694656</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -2117,23 +2140,23 @@
       <c r="G28" s="3">
         <v>0.50574713999999998</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="2">
+        <v>43</v>
+      </c>
+      <c r="I28" s="3">
         <v>6.9767444999999997E-2</v>
       </c>
-      <c r="I28" s="3">
+      <c r="J28" s="3">
         <v>0.97674417000000002</v>
       </c>
-      <c r="J28" s="3">
+      <c r="K28" s="3">
         <v>0.86046511000000003</v>
-      </c>
-      <c r="K28" s="2">
-        <v>43</v>
       </c>
       <c r="L28" s="3">
         <v>9.9667776000000007E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -2155,23 +2178,23 @@
       <c r="G29" s="3">
         <v>0.24281150000000001</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="2">
+        <v>882</v>
+      </c>
+      <c r="I29" s="3">
         <v>0.71541953000000003</v>
       </c>
-      <c r="I29" s="3">
+      <c r="J29" s="3">
         <v>0.97845804999999997</v>
       </c>
-      <c r="J29" s="3">
+      <c r="K29" s="3">
         <v>0.92849033999999997</v>
-      </c>
-      <c r="K29" s="2">
-        <v>882</v>
       </c>
       <c r="L29" s="3">
         <v>0.26879627</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
@@ -2193,23 +2216,23 @@
       <c r="G30" s="3">
         <v>0.27391305999999999</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="2">
+        <v>220</v>
+      </c>
+      <c r="I30" s="3">
         <v>7.7272727999999999E-2</v>
       </c>
-      <c r="I30" s="3">
+      <c r="J30" s="3">
         <v>0.96363633999999998</v>
       </c>
-      <c r="J30" s="3">
+      <c r="K30" s="3">
         <v>0.98636365000000004</v>
-      </c>
-      <c r="K30" s="2">
-        <v>220</v>
       </c>
       <c r="L30" s="3">
         <v>2.425107E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
@@ -2231,23 +2254,23 @@
       <c r="G31" s="3">
         <v>0.37211156000000001</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="2">
+        <v>373</v>
+      </c>
+      <c r="I31" s="3">
         <v>0.32975870000000002</v>
       </c>
-      <c r="I31" s="3">
+      <c r="J31" s="3">
         <v>0.98123324000000001</v>
       </c>
-      <c r="J31" s="3">
+      <c r="K31" s="3">
         <v>0.96782838999999998</v>
-      </c>
-      <c r="K31" s="2">
-        <v>373</v>
       </c>
       <c r="L31" s="3">
         <v>0.10022271000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
@@ -2269,23 +2292,23 @@
       <c r="G32" s="3">
         <v>0.30848177999999998</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="2">
+        <v>2018</v>
+      </c>
+      <c r="I32" s="3">
         <v>0.60753219999999997</v>
       </c>
-      <c r="I32" s="3">
+      <c r="J32" s="3">
         <v>0.98810703</v>
       </c>
-      <c r="J32" s="3">
+      <c r="K32" s="3">
         <v>0.96283448000000005</v>
-      </c>
-      <c r="K32" s="2">
-        <v>2018</v>
       </c>
       <c r="L32" s="3">
         <v>0.21646135999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
@@ -2307,23 +2330,23 @@
       <c r="G33" s="3">
         <v>0.34798002</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="2">
+        <v>1924</v>
+      </c>
+      <c r="I33" s="3">
         <v>0.60498958999999997</v>
       </c>
-      <c r="I33" s="3">
+      <c r="J33" s="3">
         <v>0.97453224999999999</v>
       </c>
-      <c r="J33" s="3">
+      <c r="K33" s="3">
         <v>0.95634096999999996</v>
-      </c>
-      <c r="K33" s="2">
-        <v>1924</v>
       </c>
       <c r="L33" s="3">
         <v>0.22725275</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
@@ -2345,23 +2368,23 @@
       <c r="G34" s="3">
         <v>0.36249101</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="2">
+        <v>1102</v>
+      </c>
+      <c r="I34" s="3">
         <v>0.42014518000000001</v>
       </c>
-      <c r="I34" s="3">
+      <c r="J34" s="3">
         <v>0.96733212000000002</v>
       </c>
-      <c r="J34" s="3">
+      <c r="K34" s="3">
         <v>0.89292198</v>
-      </c>
-      <c r="K34" s="2">
-        <v>1102</v>
       </c>
       <c r="L34" s="3">
         <v>0.14921875000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -2383,23 +2406,23 @@
       <c r="G35" s="3">
         <v>0.32260227000000002</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H35" s="2">
+        <v>401</v>
+      </c>
+      <c r="I35" s="3">
         <v>0.13715711</v>
       </c>
-      <c r="I35" s="3">
+      <c r="J35" s="3">
         <v>0.98503739000000001</v>
       </c>
-      <c r="J35" s="3">
+      <c r="K35" s="3">
         <v>0.92269325000000002</v>
-      </c>
-      <c r="K35" s="2">
-        <v>401</v>
       </c>
       <c r="L35" s="3">
         <v>3.4188035999999998E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
@@ -2421,23 +2444,23 @@
       <c r="G36" s="3">
         <v>0.41904569000000003</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H36" s="2">
+        <v>1781</v>
+      </c>
+      <c r="I36" s="3">
         <v>0.69006175000000003</v>
       </c>
-      <c r="I36" s="3">
+      <c r="J36" s="3">
         <v>0.97810220999999997</v>
       </c>
-      <c r="J36" s="3">
+      <c r="K36" s="3">
         <v>0.96294217999999998</v>
-      </c>
-      <c r="K36" s="2">
-        <v>1781</v>
       </c>
       <c r="L36" s="3">
         <v>0.23375098</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>34</v>
       </c>
@@ -2459,23 +2482,23 @@
       <c r="G37" s="3">
         <v>0.31162789000000002</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37" s="2">
+        <v>53</v>
+      </c>
+      <c r="I37" s="3">
         <v>0.35849056000000001</v>
       </c>
-      <c r="I37" s="3">
+      <c r="J37" s="3">
         <v>1</v>
       </c>
-      <c r="J37" s="3">
+      <c r="K37" s="3">
         <v>0.98113209000000001</v>
-      </c>
-      <c r="K37" s="2">
-        <v>53</v>
       </c>
       <c r="L37" s="3">
         <v>8.9430890999999998E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>35</v>
       </c>
@@ -2497,23 +2520,23 @@
       <c r="G38" s="3">
         <v>0.34849212000000002</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="2">
+        <v>867</v>
+      </c>
+      <c r="I38" s="3">
         <v>0.73702425000000005</v>
       </c>
-      <c r="I38" s="3">
+      <c r="J38" s="3">
         <v>0.96424454000000004</v>
       </c>
-      <c r="J38" s="3">
+      <c r="K38" s="3">
         <v>0.88119954</v>
-      </c>
-      <c r="K38" s="2">
-        <v>867</v>
       </c>
       <c r="L38" s="3">
         <v>0.28402659000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>36</v>
       </c>
@@ -2535,23 +2558,23 @@
       <c r="G39" s="3">
         <v>0.14705883</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="2">
+        <v>85</v>
+      </c>
+      <c r="I39" s="3">
         <v>3.5294118999999999E-2</v>
       </c>
-      <c r="I39" s="3">
+      <c r="J39" s="3">
         <v>0.95238096000000005</v>
       </c>
-      <c r="J39" s="3">
+      <c r="K39" s="3">
         <v>0.72941177999999995</v>
-      </c>
-      <c r="K39" s="2">
-        <v>85</v>
       </c>
       <c r="L39" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>37</v>
       </c>
@@ -2573,23 +2596,23 @@
       <c r="G40" s="3">
         <v>0.27269780999999998</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="2">
+        <v>1240</v>
+      </c>
+      <c r="I40" s="3">
         <v>0.61854838999999995</v>
       </c>
-      <c r="I40" s="3">
+      <c r="J40" s="3">
         <v>0.96048385000000003</v>
       </c>
-      <c r="J40" s="3">
+      <c r="K40" s="3">
         <v>0.89596772000000002</v>
-      </c>
-      <c r="K40" s="2">
-        <v>1240</v>
       </c>
       <c r="L40" s="3">
         <v>0.22284309999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>38</v>
       </c>
@@ -2611,23 +2634,23 @@
       <c r="G41" s="3">
         <v>0.29186842000000002</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="2">
+        <v>5581</v>
+      </c>
+      <c r="I41" s="3">
         <v>0.48665114999999998</v>
       </c>
-      <c r="I41" s="3">
+      <c r="J41" s="3">
         <v>0.97473573999999996</v>
       </c>
-      <c r="J41" s="3">
+      <c r="K41" s="3">
         <v>0.94535029000000004</v>
-      </c>
-      <c r="K41" s="2">
-        <v>5581</v>
       </c>
       <c r="L41" s="3">
         <v>0.16360073999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
@@ -2649,23 +2672,23 @@
       <c r="G42" s="3">
         <v>0.21029411000000001</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="2">
+        <v>157</v>
+      </c>
+      <c r="I42" s="3">
         <v>8.2802549000000003E-2</v>
       </c>
-      <c r="I42" s="3">
+      <c r="J42" s="3">
         <v>0.99363058999999998</v>
       </c>
-      <c r="J42" s="3">
+      <c r="K42" s="3">
         <v>0.90445858000000001</v>
-      </c>
-      <c r="K42" s="2">
-        <v>157</v>
       </c>
       <c r="L42" s="3">
         <v>1.5748030999999999E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>40</v>
       </c>
@@ -2687,23 +2710,23 @@
       <c r="G43" s="3">
         <v>0.31034482000000002</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="2">
+        <v>651</v>
+      </c>
+      <c r="I43" s="3">
         <v>0.27649769000000002</v>
       </c>
-      <c r="I43" s="3">
+      <c r="J43" s="3">
         <v>0.96620583999999998</v>
       </c>
-      <c r="J43" s="3">
+      <c r="K43" s="3">
         <v>0.95545316000000002</v>
-      </c>
-      <c r="K43" s="2">
-        <v>651</v>
       </c>
       <c r="L43" s="3">
         <v>9.6017696E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>41</v>
       </c>
@@ -2725,23 +2748,23 @@
       <c r="G44" s="3">
         <v>0.27313974000000002</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="2">
+        <v>960</v>
+      </c>
+      <c r="I44" s="3">
         <v>0.59479165000000001</v>
       </c>
-      <c r="I44" s="3">
+      <c r="J44" s="3">
         <v>0.98229164000000002</v>
       </c>
-      <c r="J44" s="3">
+      <c r="K44" s="3">
         <v>0.95724714</v>
-      </c>
-      <c r="K44" s="2">
-        <v>960</v>
       </c>
       <c r="L44" s="3">
         <v>0.23801321</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>42</v>
       </c>
@@ -2763,23 +2786,23 @@
       <c r="G45" s="3">
         <v>0.41294965</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="2">
+        <v>161</v>
+      </c>
+      <c r="I45" s="3">
         <v>0.13664596000000001</v>
-      </c>
-      <c r="I45" s="3">
-        <v>0.97515529000000001</v>
       </c>
       <c r="J45" s="3">
         <v>0.97515529000000001</v>
       </c>
-      <c r="K45" s="2">
-        <v>161</v>
+      <c r="K45" s="3">
+        <v>0.97515529000000001</v>
       </c>
       <c r="L45" s="3">
         <v>3.4916200000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>43</v>
       </c>
@@ -2801,29 +2824,27 @@
       <c r="G46" s="3">
         <v>0.36909871999999999</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="2">
+        <v>66</v>
+      </c>
+      <c r="I46" s="3">
         <v>0</v>
       </c>
-      <c r="I46" s="3">
+      <c r="J46" s="3">
         <v>0.98484850000000002</v>
       </c>
-      <c r="J46" s="3">
+      <c r="K46" s="3">
         <v>0.90909094000000001</v>
-      </c>
-      <c r="K46" s="2">
-        <v>66</v>
       </c>
       <c r="L46" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>59</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B47" s="2"/>
       <c r="C47" s="3">
         <v>0.40793045</v>
       </c>
@@ -2839,25 +2860,39 @@
       <c r="G47" s="3">
         <v>0.32880854999999998</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="2">
+        <v>45238</v>
+      </c>
+      <c r="I47" s="3">
         <v>0.56054645999999997</v>
       </c>
-      <c r="I47" s="3">
+      <c r="J47" s="3">
         <v>0.97760683000000004</v>
       </c>
-      <c r="J47" s="3">
+      <c r="K47" s="3">
         <v>0.93663775999999999</v>
-      </c>
-      <c r="K47" s="2">
-        <v>45238</v>
       </c>
       <c r="L47" s="3">
         <v>0.19790524000000001</v>
       </c>
     </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="L1:L2"/>
+  <mergeCells count="7">
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="F1:G1"/>

</xml_diff>